<commit_message>
26/10/23 04:30 latest update upload by ritik
</commit_message>
<xml_diff>
--- a/mongodb_Seras_Structure/uploads/Quiz_Question.xlsx
+++ b/mongodb_Seras_Structure/uploads/Quiz_Question.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hp\Desktop\SERAS-PROJECT\GIT_ONLINE_EXAM\OnlineExam\mongodb_Seras_Structure\uploads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7305"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -28,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="195">
   <si>
     <t>SubjectID</t>
   </si>
@@ -382,13 +387,244 @@
   </si>
   <si>
     <t>Sardar Patel</t>
+  </si>
+  <si>
+    <t>What is your name?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Rahul</t>
+  </si>
+  <si>
+    <t>What is the opposite of "happy"?</t>
+  </si>
+  <si>
+    <t>Angry</t>
+  </si>
+  <si>
+    <t>Sad</t>
+  </si>
+  <si>
+    <t>Excited</t>
+  </si>
+  <si>
+    <t>Joyful</t>
+  </si>
+  <si>
+    <t>Choose the correctly spelled word:</t>
+  </si>
+  <si>
+    <t>Apearence</t>
+  </si>
+  <si>
+    <t>Aparance</t>
+  </si>
+  <si>
+    <t>Appearance</t>
+  </si>
+  <si>
+    <t>Appereance</t>
+  </si>
+  <si>
+    <t>Which of the following is a synonym for "quick"?</t>
+  </si>
+  <si>
+    <t>Slow</t>
+  </si>
+  <si>
+    <t>Fast</t>
+  </si>
+  <si>
+    <t>Lazy</t>
+  </si>
+  <si>
+    <t>Hasty</t>
+  </si>
+  <si>
+    <t>What is the plural form of "child"?</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Childs</t>
+  </si>
+  <si>
+    <t>Childes</t>
+  </si>
+  <si>
+    <t>Childen</t>
+  </si>
+  <si>
+    <t>Complete the sentence: "She plays the piano ____."</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>with</t>
+  </si>
+  <si>
+    <t>on</t>
+  </si>
+  <si>
+    <t>at</t>
+  </si>
+  <si>
+    <t>Identify the subject in the sentence: "The cat chased the mouse."</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>cat</t>
+  </si>
+  <si>
+    <t>chased</t>
+  </si>
+  <si>
+    <t>mouse</t>
+  </si>
+  <si>
+    <t>What is the past tense of the verb "run"?</t>
+  </si>
+  <si>
+    <t>Runned</t>
+  </si>
+  <si>
+    <t>Ran</t>
+  </si>
+  <si>
+    <t>Running</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Which of the following is an adverb?</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Quickly</t>
+  </si>
+  <si>
+    <t>Table</t>
+  </si>
+  <si>
+    <t>Dog</t>
+  </si>
+  <si>
+    <t>What is the superlative form of "good"?</t>
+  </si>
+  <si>
+    <t>Goodest</t>
+  </si>
+  <si>
+    <t>Better</t>
+  </si>
+  <si>
+    <t>Best</t>
+  </si>
+  <si>
+    <t>Well</t>
+  </si>
+  <si>
+    <t>What is 1 + 1?</t>
+  </si>
+  <si>
+    <t>Solve for x: 2x + 5 = 15.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x = 7</t>
+  </si>
+  <si>
+    <t>x = 8</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x = 5</t>
+  </si>
+  <si>
+    <t>x = 10</t>
+  </si>
+  <si>
+    <t>What is the square root of 16?</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>If a rectangle has a length of 8 units and a width of 3 units, what is its area?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24 square units</t>
+  </si>
+  <si>
+    <t>11 square units</t>
+  </si>
+  <si>
+    <t>15 square units</t>
+  </si>
+  <si>
+    <t>21 square units</t>
+  </si>
+  <si>
+    <t>What is 10% of 80?</t>
+  </si>
+  <si>
+    <t>If a train travels at a speed of 60 km/h for 3 hours, how far does it travel?</t>
+  </si>
+  <si>
+    <t>20 km</t>
+  </si>
+  <si>
+    <t>180 km</t>
+  </si>
+  <si>
+    <t>240 km</t>
+  </si>
+  <si>
+    <t>What is the next number in the sequence: 2, 4, 6, 8, ___?</t>
+  </si>
+  <si>
+    <t>If the sum of two numbers is 12, and one of the numbers is 5, what is the other number?</t>
+  </si>
+  <si>
+    <t>How many degrees are in a right angle?</t>
+  </si>
+  <si>
+    <t>45 degrees</t>
+  </si>
+  <si>
+    <t>90 degrees</t>
+  </si>
+  <si>
+    <t>180 degrees</t>
+  </si>
+  <si>
+    <t>360 degrees</t>
+  </si>
+  <si>
+    <t>What is the perimeter of a square with a side length of 7 units?</t>
+  </si>
+  <si>
+    <t>14 units</t>
+  </si>
+  <si>
+    <t>21 units</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28 units</t>
+  </si>
+  <si>
+    <t>35 units</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="4">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,6 +650,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FFD1D5DB"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -457,7 +705,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -474,6 +722,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -746,33 +996,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="C31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="18.85546875" customWidth="1"/>
-    <col min="3" max="3" width="70.7109375" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="16.453125" customWidth="1"/>
+    <col min="2" max="2" width="18.81640625" customWidth="1"/>
+    <col min="3" max="3" width="70.7265625" customWidth="1"/>
+    <col min="4" max="4" width="25.7265625" customWidth="1"/>
+    <col min="5" max="5" width="22.7265625" customWidth="1"/>
     <col min="6" max="6" width="23" customWidth="1"/>
-    <col min="7" max="7" width="24.7109375" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="24.7265625" customWidth="1"/>
+    <col min="8" max="8" width="15.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="26.25">
+    <row r="1" spans="1:8" ht="26" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -798,7 +1048,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -824,7 +1074,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -850,7 +1100,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -876,7 +1126,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -902,7 +1152,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -928,7 +1178,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -954,7 +1204,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>1</v>
       </c>
@@ -980,7 +1230,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>4</v>
       </c>
@@ -1006,7 +1256,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>5</v>
       </c>
@@ -1032,7 +1282,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>6</v>
       </c>
@@ -1058,7 +1308,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>7</v>
       </c>
@@ -1084,7 +1334,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1110,7 +1360,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="17.25">
+    <row r="14" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A14" s="3" t="s">
         <v>1</v>
       </c>
@@ -1136,7 +1386,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="17.25">
+    <row r="15" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A15" s="3" t="s">
         <v>1</v>
       </c>
@@ -1162,7 +1412,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="17.25">
+    <row r="16" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A16" s="3" t="s">
         <v>1</v>
       </c>
@@ -1188,7 +1438,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="17.25">
+    <row r="17" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A17" s="3" t="s">
         <v>4</v>
       </c>
@@ -1214,7 +1464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="17.25">
+    <row r="18" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
@@ -1240,7 +1490,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="17.25">
+    <row r="19" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A19" s="3" t="s">
         <v>4</v>
       </c>
@@ -1266,7 +1516,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="17.25">
+    <row r="20" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A20" s="3" t="s">
         <v>5</v>
       </c>
@@ -1292,7 +1542,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="17.25">
+    <row r="21" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A21" s="3" t="s">
         <v>5</v>
       </c>
@@ -1318,7 +1568,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="17.25">
+    <row r="22" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A22" s="3" t="s">
         <v>5</v>
       </c>
@@ -1344,7 +1594,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="17.25">
+    <row r="23" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A23" s="3" t="s">
         <v>6</v>
       </c>
@@ -1370,7 +1620,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="17.25">
+    <row r="24" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A24" s="3" t="s">
         <v>6</v>
       </c>
@@ -1396,7 +1646,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="17.25">
+    <row r="25" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A25" s="3" t="s">
         <v>6</v>
       </c>
@@ -1422,7 +1672,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="17.25">
+    <row r="26" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A26" s="3" t="s">
         <v>7</v>
       </c>
@@ -1448,7 +1698,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="17.25">
+    <row r="27" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A27" s="3" t="s">
         <v>7</v>
       </c>
@@ -1474,7 +1724,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="17.25">
+    <row r="28" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A28" s="3" t="s">
         <v>7</v>
       </c>
@@ -1500,7 +1750,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="17.25">
+    <row r="29" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -1526,7 +1776,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="17.25">
+    <row r="30" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1552,7 +1802,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="17.25">
+    <row r="31" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
@@ -1578,7 +1828,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="17.25">
+    <row r="32" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
       <c r="A32" s="3" t="s">
         <v>8</v>
       </c>
@@ -1604,115 +1854,577 @@
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
-      <c r="B33" s="3"/>
-    </row>
-    <row r="34" spans="2:2">
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="2:2">
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="2:2">
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="2:2">
-      <c r="B37" s="3"/>
-    </row>
-    <row r="38" spans="2:2">
-      <c r="B38" s="3"/>
-    </row>
-    <row r="39" spans="2:2">
-      <c r="B39" s="3"/>
-    </row>
-    <row r="40" spans="2:2">
-      <c r="B40" s="3"/>
-    </row>
-    <row r="41" spans="2:2">
-      <c r="B41" s="3"/>
-    </row>
-    <row r="42" spans="2:2">
-      <c r="B42" s="3"/>
-    </row>
-    <row r="43" spans="2:2">
-      <c r="B43" s="3"/>
-    </row>
-    <row r="44" spans="2:2">
-      <c r="B44" s="3"/>
-    </row>
-    <row r="45" spans="2:2">
-      <c r="B45" s="3"/>
-    </row>
-    <row r="46" spans="2:2">
-      <c r="B46" s="3"/>
-    </row>
-    <row r="47" spans="2:2">
-      <c r="B47" s="3"/>
-    </row>
-    <row r="48" spans="2:2">
-      <c r="B48" s="3"/>
-    </row>
-    <row r="49" spans="2:2">
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="2:2">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="2:2">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="2:2">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="2:2">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="2:2">
+    <row r="33" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A33" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B33" s="3">
+        <v>32</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A34" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B34" s="3">
+        <v>33</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A35" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3">
+        <v>34</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="F35" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="3">
+        <v>35</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F36" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A37" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3">
+        <v>36</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F37" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A38" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B38" s="3">
+        <v>37</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B39" s="3">
+        <v>38</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A40" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="3">
+        <v>39</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="D40" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A41" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B41" s="3">
+        <v>40</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>156</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="H41" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A42" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B42" s="3">
+        <v>41</v>
+      </c>
+      <c r="C42" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D42" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H42" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B43" s="3">
+        <v>42</v>
+      </c>
+      <c r="C43" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="D43">
+        <v>3</v>
+      </c>
+      <c r="E43">
+        <v>11</v>
+      </c>
+      <c r="F43">
+        <v>2</v>
+      </c>
+      <c r="G43" s="6">
+        <v>33</v>
+      </c>
+      <c r="H43" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A44" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B44" s="3">
+        <v>43</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="F44" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="17.5" x14ac:dyDescent="0.45">
+      <c r="A45" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B45" s="3">
+        <v>44</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45">
+        <v>4</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="G45">
+        <v>5</v>
+      </c>
+      <c r="H45" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B46" s="3">
+        <v>45</v>
+      </c>
+      <c r="C46" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>177</v>
+      </c>
+      <c r="H46" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B47" s="3">
+        <v>46</v>
+      </c>
+      <c r="C47" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="D47">
+        <v>8</v>
+      </c>
+      <c r="E47">
+        <v>800</v>
+      </c>
+      <c r="F47">
+        <v>0.8</v>
+      </c>
+      <c r="G47">
+        <v>80</v>
+      </c>
+      <c r="H47" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B48" s="3">
+        <v>47</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>179</v>
+      </c>
+      <c r="D48" t="s">
+        <v>180</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="H48" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A49" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B49" s="3">
+        <v>48</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D49">
+        <v>9</v>
+      </c>
+      <c r="E49">
+        <v>10</v>
+      </c>
+      <c r="F49">
+        <v>12</v>
+      </c>
+      <c r="G49">
+        <v>14</v>
+      </c>
+      <c r="H49" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B50" s="3">
+        <v>49</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>184</v>
+      </c>
+      <c r="D50">
+        <v>6</v>
+      </c>
+      <c r="E50" s="6">
+        <v>7</v>
+      </c>
+      <c r="F50">
+        <v>8</v>
+      </c>
+      <c r="G50" s="6">
+        <v>9</v>
+      </c>
+      <c r="H50" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3">
+        <v>50</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>186</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="F51" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="G51" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="H51" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B52" s="3">
+        <v>51</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="F52" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="G52" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="H52" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B53" s="3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B54" s="3"/>
     </row>
-    <row r="55" spans="2:2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B55" s="3"/>
     </row>
-    <row r="56" spans="2:2">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B56" s="3"/>
     </row>
-    <row r="57" spans="2:2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B57" s="3"/>
     </row>
-    <row r="58" spans="2:2">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B58" s="3"/>
     </row>
-    <row r="59" spans="2:2">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B59" s="3"/>
     </row>
-    <row r="60" spans="2:2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B60" s="3"/>
     </row>
-    <row r="61" spans="2:2">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B61" s="3"/>
     </row>
-    <row r="62" spans="2:2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B62" s="3"/>
     </row>
-    <row r="63" spans="2:2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B63" s="3"/>
     </row>
-    <row r="64" spans="2:2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B64" s="3"/>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="3"/>
     </row>
-    <row r="66" spans="2:2">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="3"/>
     </row>
-    <row r="67" spans="2:2">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="3"/>
     </row>
-    <row r="68" spans="2:2">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="3"/>
     </row>
-    <row r="69" spans="2:2">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="3"/>
     </row>
   </sheetData>

</xml_diff>